<commit_message>
added popups, started on slider buttons
</commit_message>
<xml_diff>
--- a/chapter1/data/spatioTemporalData.xlsx
+++ b/chapter1/data/spatioTemporalData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medst\Dropbox\Grad School\Fall 2023\Geog575\unit-2\unit-2\chapter1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8D3FFC-8EAA-4802-82AD-05F234B0CAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B6C237-2E2B-45A2-851C-6EBB33405947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{9F1ACF37-6E63-439C-AC7F-05EEE91F7D92}"/>
   </bookViews>
@@ -98,34 +98,34 @@
     <t>Edina</t>
   </si>
   <si>
+    <t>AvgComTime2014</t>
+  </si>
+  <si>
+    <t>AvgComTime2016</t>
+  </si>
+  <si>
+    <t>AvgComTime2018</t>
+  </si>
+  <si>
+    <t>AvgComTime2013</t>
+  </si>
+  <si>
+    <t>AvgComTime2015</t>
+  </si>
+  <si>
+    <t>AvgComTime2017</t>
+  </si>
+  <si>
+    <t>AvgComTime2019</t>
+  </si>
+  <si>
+    <t>AvgComTime2012</t>
+  </si>
+  <si>
+    <t>AvgComTime2011</t>
+  </si>
+  <si>
     <t>AvgComTime2010</t>
-  </si>
-  <si>
-    <t>AvgComTime2012</t>
-  </si>
-  <si>
-    <t>AvgComTime2014</t>
-  </si>
-  <si>
-    <t>AvgComTime2016</t>
-  </si>
-  <si>
-    <t>AvgComTime2018</t>
-  </si>
-  <si>
-    <t>AvgComTime2011</t>
-  </si>
-  <si>
-    <t>AvgComTime2013</t>
-  </si>
-  <si>
-    <t>AvgComTime2015</t>
-  </si>
-  <si>
-    <t>AvgComTime2017</t>
-  </si>
-  <si>
-    <t>AvgComTime2019</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -507,34 +507,34 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
         <v>26</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.45">
@@ -1202,5 +1202,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>